<commit_message>
easy stages enemy added
</commit_message>
<xml_diff>
--- a/Stages Updated pero di pa tapos.xlsx
+++ b/Stages Updated pero di pa tapos.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kotaro\Desktop\DESKTOP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dayne Helbano\Desktop\FV-Adventure\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
   <si>
     <t>Stage Name</t>
   </si>
@@ -117,12 +117,33 @@
   </si>
   <si>
     <t>The Palace of the INSECTcure insect queen.  It consists of 3 identical places.</t>
+  </si>
+  <si>
+    <t>Mole</t>
+  </si>
+  <si>
+    <t>Mice</t>
+  </si>
+  <si>
+    <t>Prideful Worm</t>
+  </si>
+  <si>
+    <t>Beetle 1</t>
+  </si>
+  <si>
+    <t>Beetle 2</t>
+  </si>
+  <si>
+    <t>Beetle 3</t>
+  </si>
+  <si>
+    <t>Queen Bitter Gourd</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -177,7 +198,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -214,6 +235,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -519,10 +543,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -672,10 +696,45 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="21" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="22" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="2"/>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A23" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A26" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
new enemies rendered to the game, easy stages ready for testing
</commit_message>
<xml_diff>
--- a/Stages Updated pero di pa tapos.xlsx
+++ b/Stages Updated pero di pa tapos.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dayne Helbano\Desktop\FV-Adventure\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kotaro\Documents\FV-Adventure\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="53">
   <si>
     <t>Stage Name</t>
   </si>
@@ -74,15 +74,6 @@
     <t>Insect Queen</t>
   </si>
   <si>
-    <t>Big Snail</t>
-  </si>
-  <si>
-    <t>Armored Caterpillar</t>
-  </si>
-  <si>
-    <t>3 beetles</t>
-  </si>
-  <si>
     <t>Insect Palace</t>
   </si>
   <si>
@@ -128,9 +119,6 @@
     <t>Prideful Worm</t>
   </si>
   <si>
-    <t>Beetle 1</t>
-  </si>
-  <si>
     <t>Beetle 2</t>
   </si>
   <si>
@@ -138,13 +126,67 @@
   </si>
   <si>
     <t>Queen Bitter Gourd</t>
+  </si>
+  <si>
+    <t>mice</t>
+  </si>
+  <si>
+    <t>mole</t>
+  </si>
+  <si>
+    <t>prideful worm</t>
+  </si>
+  <si>
+    <t>boss caterpillar</t>
+  </si>
+  <si>
+    <t>boss fly</t>
+  </si>
+  <si>
+    <t>beetle 2</t>
+  </si>
+  <si>
+    <t>beetle 3</t>
+  </si>
+  <si>
+    <t>HP</t>
+  </si>
+  <si>
+    <t>Pathway</t>
+  </si>
+  <si>
+    <t>Ability</t>
+  </si>
+  <si>
+    <t>Speed</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>Normal</t>
+  </si>
+  <si>
+    <t>Land</t>
+  </si>
+  <si>
+    <t>boss grasshopper</t>
+  </si>
+  <si>
+    <t>HIgh</t>
+  </si>
+  <si>
+    <t>Air</t>
+  </si>
+  <si>
+    <t>Fast</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -165,8 +207,15 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -185,6 +234,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -198,7 +259,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -236,7 +297,32 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -543,19 +629,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D26"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21:XFD21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="28" style="1" customWidth="1"/>
     <col min="2" max="2" width="56.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="56.5703125" style="4" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="1"/>
+    <col min="3" max="3" width="20.140625" style="15" customWidth="1"/>
+    <col min="4" max="4" width="35.5703125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="2" customFormat="1" ht="15" x14ac:dyDescent="0.25">
@@ -565,11 +652,11 @@
       <c r="B1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="11" t="s">
         <v>14</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -582,42 +669,51 @@
         <v>13</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3" s="8"/>
+        <v>19</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="4" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="8"/>
+        <v>20</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="5" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" s="8"/>
+        <v>21</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="6" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6" s="8"/>
+        <v>22</v>
+      </c>
+      <c r="C6" s="19" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="7" spans="1:4" s="13" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="12"/>
+      <c r="C7" s="16"/>
       <c r="D7" s="14"/>
     </row>
     <row r="8" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
@@ -625,19 +721,21 @@
         <v>7</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" s="8"/>
+        <v>23</v>
+      </c>
+      <c r="C8" s="20" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="9" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>18</v>
+        <v>24</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
@@ -645,43 +743,43 @@
         <v>10</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>19</v>
+        <v>25</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="6"/>
       <c r="B11" s="7"/>
-      <c r="C11" s="13"/>
+      <c r="C11" s="16"/>
     </row>
     <row r="12" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B12" s="7"/>
-      <c r="C12" s="13"/>
+      <c r="C12" s="16"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
         <v>9</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>17</v>
+        <v>26</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="C14" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="16" t="s">
         <v>15</v>
       </c>
     </row>
@@ -690,49 +788,110 @@
         <v>11</v>
       </c>
       <c r="B15" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B18" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="C18" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E18" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="G18" s="18"/>
+    </row>
+    <row r="19" spans="1:7" s="21" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="D19" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="E19" s="21" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" s="21" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="D20" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="E20" s="21" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" s="21" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="C21" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="D21" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="E21" s="21" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" s="21" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="C22" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="D22" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="E22" s="21" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C15" s="8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24" s="8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25" s="8" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" s="8" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" s="8" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="1:1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="15" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A25" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" s="8" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>

<commit_message>
beetle 2 boss added
</commit_message>
<xml_diff>
--- a/Stages Updated pero di pa tapos.xlsx
+++ b/Stages Updated pero di pa tapos.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="56">
   <si>
     <t>Stage Name</t>
   </si>
@@ -180,6 +180,15 @@
   </si>
   <si>
     <t>Fast</t>
+  </si>
+  <si>
+    <t>Slow</t>
+  </si>
+  <si>
+    <t>Extremely High</t>
+  </si>
+  <si>
+    <t>Very High</t>
   </si>
 </sst>
 </file>
@@ -631,8 +640,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:XFD21"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23:XFD24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -865,34 +874,80 @@
         <v>52</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23" s="8" t="s">
+    <row r="23" spans="1:7" s="21" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="21" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A24" s="8" t="s">
+      <c r="C23" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="D23" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="E23" s="21" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" s="21" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="21" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A25" s="8" t="s">
+      <c r="C24" s="22"/>
+      <c r="D24" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="E24" s="21" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" s="21" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="21" t="s">
         <v>32</v>
+      </c>
+      <c r="C25" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="D25" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="E25" s="21" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" s="8" t="s">
         <v>33</v>
       </c>
+      <c r="D26" s="4" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" s="8" t="s">
         <v>34</v>
       </c>
+      <c r="C27" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" s="8" t="s">
         <v>16</v>
+      </c>
+      <c r="C28" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
all insects added docu edited but not finished
</commit_message>
<xml_diff>
--- a/Stages Updated pero di pa tapos.xlsx
+++ b/Stages Updated pero di pa tapos.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="56">
   <si>
     <t>Stage Name</t>
   </si>
@@ -641,7 +641,7 @@
   <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23:XFD24"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -918,8 +918,14 @@
       <c r="A26" s="8" t="s">
         <v>33</v>
       </c>
+      <c r="C26" s="15" t="s">
+        <v>48</v>
+      </c>
       <c r="D26" s="4" t="s">
         <v>55</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
designing of level 7-1
</commit_message>
<xml_diff>
--- a/Stages Updated pero di pa tapos.xlsx
+++ b/Stages Updated pero di pa tapos.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="60">
   <si>
     <t>Stage Name</t>
   </si>
@@ -170,9 +170,6 @@
     <t>Land</t>
   </si>
   <si>
-    <t>boss grasshopper</t>
-  </si>
-  <si>
     <t>HIgh</t>
   </si>
   <si>
@@ -189,13 +186,28 @@
   </si>
   <si>
     <t>Very High</t>
+  </si>
+  <si>
+    <t>Prideful worm</t>
+  </si>
+  <si>
+    <t>beetle 1</t>
+  </si>
+  <si>
+    <t>queen bitter gourd</t>
+  </si>
+  <si>
+    <t>insect queen</t>
+  </si>
+  <si>
+    <t>Beetle 1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -218,6 +230,12 @@
     </font>
     <font>
       <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
@@ -268,7 +286,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -333,6 +351,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -638,10 +659,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26:XFD26"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -714,7 +735,7 @@
         <v>22</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="13" customFormat="1" ht="15" x14ac:dyDescent="0.2">
@@ -840,7 +861,7 @@
         <v>48</v>
       </c>
       <c r="D20" s="23" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E20" s="21" t="s">
         <v>47</v>
@@ -851,18 +872,18 @@
         <v>39</v>
       </c>
       <c r="C21" s="22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D21" s="23" t="s">
         <v>47</v>
       </c>
       <c r="E21" s="21" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="22" spans="1:7" s="21" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="24" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="C22" s="22" t="s">
         <v>48</v>
@@ -885,7 +906,7 @@
         <v>46</v>
       </c>
       <c r="E23" s="21" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="24" spans="1:7" s="21" customFormat="1" x14ac:dyDescent="0.2">
@@ -894,10 +915,10 @@
       </c>
       <c r="C24" s="22"/>
       <c r="D24" s="23" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E24" s="21" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="25" spans="1:7" s="21" customFormat="1" x14ac:dyDescent="0.2">
@@ -908,7 +929,7 @@
         <v>48</v>
       </c>
       <c r="D25" s="23" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E25" s="21" t="s">
         <v>47</v>
@@ -922,7 +943,7 @@
         <v>48</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>47</v>
@@ -936,7 +957,7 @@
         <v>48</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>47</v>
@@ -950,10 +971,50 @@
         <v>48</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="A31" s="25" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+      <c r="A32" s="25" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A33" s="25" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A34" s="25" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A35" s="25" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A36" s="25" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A37" s="25" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A38" s="25" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>